<commit_message>
Divisão de ROE e ROIC 2
</commit_message>
<xml_diff>
--- a/Fii_Tij_Hibrid_Mágicas.xlsx
+++ b/Fii_Tij_Hibrid_Mágicas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>Papel</t>
   </si>
@@ -64,10 +64,16 @@
     <t>Score</t>
   </si>
   <si>
+    <t>BTAL11</t>
+  </si>
+  <si>
+    <t>BRCR11</t>
+  </si>
+  <si>
     <t>RZAT11</t>
   </si>
   <si>
-    <t>BTAL11</t>
+    <t>GALG11</t>
   </si>
   <si>
     <t>VINO11</t>
@@ -76,76 +82,67 @@
     <t>MALL11</t>
   </si>
   <si>
-    <t>BRCR11</t>
+    <t>RBRL11</t>
+  </si>
+  <si>
+    <t>HSML11</t>
+  </si>
+  <si>
+    <t>RBVA11</t>
+  </si>
+  <si>
+    <t>TEPP11</t>
+  </si>
+  <si>
+    <t>XPLG11</t>
+  </si>
+  <si>
+    <t>GGRC11</t>
   </si>
   <si>
     <t>TVRI11</t>
   </si>
   <si>
-    <t>GALG11</t>
-  </si>
-  <si>
-    <t>RBRL11</t>
-  </si>
-  <si>
-    <t>GGRC11</t>
-  </si>
-  <si>
-    <t>HSLG11</t>
-  </si>
-  <si>
-    <t>HSML11</t>
-  </si>
-  <si>
-    <t>TEPP11</t>
-  </si>
-  <si>
-    <t>RBVA11</t>
-  </si>
-  <si>
-    <t>XPLG11</t>
+    <t>VISC11</t>
   </si>
   <si>
     <t>TRXF11</t>
   </si>
   <si>
+    <t>HGBS11</t>
+  </si>
+  <si>
+    <t>HGRU11</t>
+  </si>
+  <si>
     <t>HTMX11</t>
   </si>
   <si>
     <t>LVBI11</t>
   </si>
   <si>
+    <t>ALZR11</t>
+  </si>
+  <si>
+    <t>KNRI11</t>
+  </si>
+  <si>
     <t>BRCO11</t>
   </si>
   <si>
-    <t>HGRU11</t>
-  </si>
-  <si>
-    <t>KNRI11</t>
-  </si>
-  <si>
-    <t>HGBS11</t>
+    <t>BTLG11</t>
+  </si>
+  <si>
+    <t>HSRE11</t>
   </si>
   <si>
     <t>XPML11</t>
   </si>
   <si>
-    <t>HSRE11</t>
-  </si>
-  <si>
-    <t>ALZR11</t>
-  </si>
-  <si>
-    <t>VISC11</t>
-  </si>
-  <si>
-    <t>BTLG11</t>
+    <t>Outros</t>
   </si>
   <si>
     <t>Híbrido</t>
-  </si>
-  <si>
-    <t>Outros</t>
   </si>
   <si>
     <t>Lajes Corporativas</t>
@@ -515,7 +512,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -576,49 +573,49 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2">
-        <v>95.19</v>
+        <v>75.40000000000001</v>
       </c>
       <c r="D2">
-        <v>11.76</v>
+        <v>10.26</v>
       </c>
       <c r="E2">
-        <v>11.19</v>
+        <v>12.14</v>
       </c>
       <c r="F2">
-        <v>0.9399999999999999</v>
+        <v>0.72</v>
       </c>
       <c r="G2">
-        <v>352981000</v>
+        <v>451098000</v>
       </c>
       <c r="H2">
-        <v>1126580</v>
+        <v>1066020</v>
       </c>
       <c r="I2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J2">
-        <v>1129.79</v>
+        <v>1394.03</v>
       </c>
       <c r="K2">
-        <v>112</v>
+        <v>167.71</v>
       </c>
       <c r="L2">
-        <v>9.91</v>
+        <v>12.03</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P2">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -626,49 +623,49 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3">
-        <v>78.15000000000001</v>
+        <v>59.7</v>
       </c>
       <c r="D3">
-        <v>9.9</v>
+        <v>9.390000000000001</v>
       </c>
       <c r="E3">
-        <v>10.98</v>
+        <v>9.09</v>
       </c>
       <c r="F3">
-        <v>0.74</v>
+        <v>0.61</v>
       </c>
       <c r="G3">
-        <v>467551000</v>
+        <v>1590300000</v>
       </c>
       <c r="H3">
-        <v>1100970</v>
+        <v>2291530</v>
       </c>
       <c r="I3">
         <v>9</v>
       </c>
       <c r="J3">
-        <v>1439.69</v>
+        <v>10884.2</v>
       </c>
       <c r="K3">
-        <v>167.71</v>
+        <v>1257.63</v>
       </c>
       <c r="L3">
-        <v>11.65</v>
+        <v>11.55</v>
       </c>
       <c r="M3">
+        <v>6.2</v>
+      </c>
+      <c r="N3">
         <v>0</v>
       </c>
-      <c r="N3">
-        <v>2</v>
-      </c>
       <c r="O3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P3">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -676,49 +673,49 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4">
-        <v>7.68</v>
+        <v>94.84999999999999</v>
       </c>
       <c r="D4">
-        <v>9.83</v>
+        <v>11.81</v>
       </c>
       <c r="E4">
-        <v>9.06</v>
+        <v>12.24</v>
       </c>
       <c r="F4">
-        <v>0.71</v>
+        <v>0.95</v>
       </c>
       <c r="G4">
-        <v>636106000</v>
+        <v>351720000</v>
       </c>
       <c r="H4">
-        <v>1005010</v>
+        <v>1073590</v>
       </c>
       <c r="I4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J4">
-        <v>9918.290000000001</v>
+        <v>1143.92</v>
       </c>
       <c r="K4">
-        <v>1177.61</v>
+        <v>112</v>
       </c>
       <c r="L4">
-        <v>11.87</v>
+        <v>9.789999999999999</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
+        <v>6</v>
+      </c>
+      <c r="O4">
         <v>1</v>
       </c>
-      <c r="O4">
-        <v>5</v>
-      </c>
       <c r="P4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -726,49 +723,49 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C5">
-        <v>118.17</v>
+        <v>9.07</v>
       </c>
       <c r="D5">
-        <v>18.1</v>
+        <v>10.23</v>
       </c>
       <c r="E5">
-        <v>7.8</v>
+        <v>9.449999999999999</v>
       </c>
       <c r="F5">
-        <v>0.99</v>
+        <v>0.91</v>
       </c>
       <c r="G5">
-        <v>1078260000</v>
+        <v>521392000</v>
       </c>
       <c r="H5">
-        <v>1890480</v>
+        <v>3232460</v>
       </c>
       <c r="I5">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J5">
-        <v>4339.78</v>
+        <v>4934.81</v>
       </c>
       <c r="K5">
-        <v>690.38</v>
+        <v>499.16</v>
       </c>
       <c r="L5">
-        <v>15.91</v>
+        <v>10.12</v>
       </c>
       <c r="M5">
-        <v>3.67</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P5">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -776,49 +773,49 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C6">
-        <v>60.73</v>
+        <v>8.08</v>
       </c>
       <c r="D6">
-        <v>9.23</v>
+        <v>9.34</v>
       </c>
       <c r="E6">
-        <v>8.32</v>
+        <v>8.619999999999999</v>
       </c>
       <c r="F6">
-        <v>0.61</v>
+        <v>0.75</v>
       </c>
       <c r="G6">
-        <v>1617740000</v>
+        <v>669236000</v>
       </c>
       <c r="H6">
-        <v>2478590</v>
+        <v>1021380</v>
       </c>
       <c r="I6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J6">
-        <v>10875.3</v>
+        <v>10466.3</v>
       </c>
       <c r="K6">
-        <v>1257.63</v>
+        <v>1177.61</v>
       </c>
       <c r="L6">
-        <v>11.56</v>
+        <v>11.25</v>
       </c>
       <c r="M6">
-        <v>6.2</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P6">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -829,46 +826,46 @@
         <v>44</v>
       </c>
       <c r="C7">
-        <v>98.8</v>
+        <v>118.95</v>
       </c>
       <c r="D7">
-        <v>10.13</v>
+        <v>17.98</v>
       </c>
       <c r="E7">
-        <v>2.71</v>
+        <v>7.75</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="G7">
-        <v>1572870000</v>
+        <v>1085380000</v>
       </c>
       <c r="H7">
-        <v>1116620</v>
+        <v>1848560</v>
       </c>
       <c r="I7">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="J7">
-        <v>4070.14</v>
+        <v>4111.29</v>
       </c>
       <c r="K7">
-        <v>456.8</v>
+        <v>690.38</v>
       </c>
       <c r="L7">
-        <v>11.22</v>
+        <v>16.79</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>3.67</v>
       </c>
       <c r="N7">
         <v>9</v>
       </c>
       <c r="O7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P7">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -876,49 +873,49 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C8">
-        <v>9.210000000000001</v>
+        <v>87.59</v>
       </c>
       <c r="D8">
-        <v>10.08</v>
+        <v>8.210000000000001</v>
       </c>
       <c r="E8">
-        <v>9.300000000000001</v>
+        <v>9.359999999999999</v>
       </c>
       <c r="F8">
-        <v>1.01</v>
+        <v>0.87</v>
       </c>
       <c r="G8">
-        <v>529440000</v>
+        <v>585717000</v>
       </c>
       <c r="H8">
-        <v>2683800</v>
+        <v>963369</v>
       </c>
       <c r="I8">
         <v>5</v>
       </c>
       <c r="J8">
-        <v>5189.54</v>
+        <v>2628.54</v>
       </c>
       <c r="K8">
-        <v>499.16</v>
+        <v>268</v>
       </c>
       <c r="L8">
-        <v>9.619999999999999</v>
+        <v>10.2</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="N8">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="O8">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="P8">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -926,49 +923,49 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C9">
-        <v>89.93000000000001</v>
+        <v>96.22</v>
       </c>
       <c r="D9">
-        <v>7.99</v>
+        <v>8.82</v>
       </c>
       <c r="E9">
-        <v>8.390000000000001</v>
+        <v>8.720000000000001</v>
       </c>
       <c r="F9">
-        <v>0.85</v>
+        <v>1.01</v>
       </c>
       <c r="G9">
-        <v>601365000</v>
+        <v>1518410000</v>
       </c>
       <c r="H9">
-        <v>928983</v>
+        <v>3162110</v>
       </c>
       <c r="I9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J9">
-        <v>2659.77</v>
+        <v>10212.5</v>
       </c>
       <c r="K9">
-        <v>268</v>
+        <v>843.77</v>
       </c>
       <c r="L9">
-        <v>10.08</v>
+        <v>8.26</v>
       </c>
       <c r="M9">
-        <v>7</v>
+        <v>5.58</v>
       </c>
       <c r="N9">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="O9">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P9">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -976,49 +973,49 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C10">
-        <v>113.8</v>
+        <v>112.24</v>
       </c>
       <c r="D10">
-        <v>8.029999999999999</v>
+        <v>9.15</v>
       </c>
       <c r="E10">
-        <v>10.39</v>
+        <v>10.72</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>1.02</v>
       </c>
       <c r="G10">
-        <v>1027750000</v>
+        <v>1401350000</v>
       </c>
       <c r="H10">
-        <v>1398220</v>
+        <v>1447550</v>
       </c>
       <c r="I10">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="J10">
-        <v>1144.89</v>
+        <v>16943.5</v>
       </c>
       <c r="K10">
-        <v>117.09</v>
+        <v>1929.88</v>
       </c>
       <c r="L10">
-        <v>10.23</v>
+        <v>11.39</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>1.21</v>
       </c>
       <c r="N10">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O10">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="P10">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1026,49 +1023,49 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C11">
-        <v>97.88</v>
+        <v>93.78</v>
       </c>
       <c r="D11">
-        <v>7.74</v>
+        <v>6.8</v>
       </c>
       <c r="E11">
-        <v>8.49</v>
+        <v>7.44</v>
       </c>
       <c r="F11">
-        <v>0.9399999999999999</v>
+        <v>0.97</v>
       </c>
       <c r="G11">
-        <v>1239170000</v>
+        <v>395936000</v>
       </c>
       <c r="H11">
-        <v>952007</v>
+        <v>1200960</v>
       </c>
       <c r="I11">
         <v>5</v>
       </c>
       <c r="J11">
-        <v>2938.74</v>
+        <v>11572.1</v>
       </c>
       <c r="K11">
-        <v>250.54</v>
+        <v>950.74</v>
       </c>
       <c r="L11">
-        <v>8.529999999999999</v>
+        <v>8.220000000000001</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O11">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="P11">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1079,46 +1076,46 @@
         <v>45</v>
       </c>
       <c r="C12">
-        <v>95.51000000000001</v>
+        <v>109.9</v>
       </c>
       <c r="D12">
-        <v>8.890000000000001</v>
+        <v>7.44</v>
       </c>
       <c r="E12">
-        <v>8.779999999999999</v>
+        <v>7.29</v>
       </c>
       <c r="F12">
-        <v>1.01</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>1507210000</v>
+        <v>3254490000</v>
       </c>
       <c r="H12">
-        <v>2774930</v>
+        <v>7347820</v>
       </c>
       <c r="I12">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="J12">
-        <v>10187</v>
+        <v>2465.64</v>
       </c>
       <c r="K12">
-        <v>843.77</v>
+        <v>201.23</v>
       </c>
       <c r="L12">
-        <v>8.279999999999999</v>
+        <v>8.16</v>
       </c>
       <c r="M12">
-        <v>5.58</v>
+        <v>4.11</v>
       </c>
       <c r="N12">
+        <v>10</v>
+      </c>
+      <c r="O12">
         <v>12</v>
       </c>
-      <c r="O12">
-        <v>8</v>
-      </c>
       <c r="P12">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1126,49 +1123,49 @@
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13">
-        <v>93.33</v>
+        <v>114.58</v>
       </c>
       <c r="D13">
-        <v>6.83</v>
+        <v>7.98</v>
       </c>
       <c r="E13">
-        <v>7.48</v>
+        <v>10.32</v>
       </c>
       <c r="F13">
-        <v>0.98</v>
+        <v>1.01</v>
       </c>
       <c r="G13">
-        <v>394036000</v>
+        <v>1034790000</v>
       </c>
       <c r="H13">
-        <v>1320840</v>
+        <v>1320950</v>
       </c>
       <c r="I13">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="J13">
-        <v>11494.2</v>
+        <v>1228.31</v>
       </c>
       <c r="K13">
-        <v>950.74</v>
+        <v>117.09</v>
       </c>
       <c r="L13">
-        <v>8.27</v>
+        <v>9.529999999999999</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="O13">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="P13">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1179,43 +1176,43 @@
         <v>43</v>
       </c>
       <c r="C14">
-        <v>113</v>
+        <v>104.99</v>
       </c>
       <c r="D14">
-        <v>9.789999999999999</v>
+        <v>9.529999999999999</v>
       </c>
       <c r="E14">
-        <v>10.65</v>
+        <v>2.55</v>
       </c>
       <c r="F14">
-        <v>1.05</v>
+        <v>1.06</v>
       </c>
       <c r="G14">
-        <v>1309470000</v>
+        <v>1671410000</v>
       </c>
       <c r="H14">
-        <v>1289320</v>
+        <v>1470870</v>
       </c>
       <c r="I14">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="J14">
-        <v>17417.7</v>
+        <v>4321.89</v>
       </c>
       <c r="K14">
-        <v>1929.88</v>
+        <v>456.8</v>
       </c>
       <c r="L14">
-        <v>11.08</v>
+        <v>10.57</v>
       </c>
       <c r="M14">
-        <v>1.21</v>
+        <v>0</v>
       </c>
       <c r="N14">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="O14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P14">
         <v>24</v>
@@ -1226,49 +1223,49 @@
         <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15">
-        <v>109.99</v>
+        <v>121.72</v>
       </c>
       <c r="D15">
-        <v>7.43</v>
+        <v>6.21</v>
       </c>
       <c r="E15">
-        <v>7.28</v>
+        <v>8.289999999999999</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0.91</v>
       </c>
       <c r="G15">
-        <v>3257160000</v>
+        <v>2585780000</v>
       </c>
       <c r="H15">
-        <v>7531940</v>
+        <v>7477160</v>
       </c>
       <c r="I15">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J15">
-        <v>2513.09</v>
+        <v>4067.29</v>
       </c>
       <c r="K15">
-        <v>201.23</v>
+        <v>319.62</v>
       </c>
       <c r="L15">
-        <v>8.01</v>
+        <v>7.86</v>
       </c>
       <c r="M15">
-        <v>4.11</v>
+        <v>5.98</v>
       </c>
       <c r="N15">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="O15">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="P15">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1279,46 +1276,46 @@
         <v>42</v>
       </c>
       <c r="C16">
-        <v>112.01</v>
+        <v>111.15</v>
       </c>
       <c r="D16">
-        <v>7.77</v>
+        <v>6.76</v>
       </c>
       <c r="E16">
-        <v>9.56</v>
+        <v>9.640000000000001</v>
       </c>
       <c r="F16">
-        <v>1.08</v>
+        <v>1.03</v>
       </c>
       <c r="G16">
-        <v>1486370000</v>
+        <v>1708620000</v>
       </c>
       <c r="H16">
-        <v>7726760</v>
+        <v>10487200</v>
       </c>
       <c r="I16">
         <v>29</v>
       </c>
       <c r="J16">
-        <v>3183.52</v>
+        <v>3166.31</v>
       </c>
       <c r="K16">
         <v>326.83</v>
       </c>
       <c r="L16">
-        <v>10.27</v>
+        <v>10.32</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="O16">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="P16">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1326,49 +1323,49 @@
         <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C17">
-        <v>175.89</v>
+        <v>228</v>
       </c>
       <c r="D17">
-        <v>8.59</v>
+        <v>5.74</v>
       </c>
       <c r="E17">
+        <v>8.390000000000001</v>
+      </c>
+      <c r="F17">
+        <v>0.98</v>
+      </c>
+      <c r="G17">
+        <v>2902390000</v>
+      </c>
+      <c r="H17">
+        <v>5592940</v>
+      </c>
+      <c r="I17">
         <v>13</v>
       </c>
-      <c r="F17">
-        <v>1.36</v>
-      </c>
-      <c r="G17">
-        <v>264597000</v>
-      </c>
-      <c r="H17">
-        <v>1966040</v>
-      </c>
-      <c r="I17">
-        <v>22</v>
-      </c>
       <c r="J17">
-        <v>348.4</v>
+        <v>5313.49</v>
       </c>
       <c r="K17">
-        <v>28.08</v>
+        <v>316.98</v>
       </c>
       <c r="L17">
-        <v>8.06</v>
+        <v>5.97</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>5.97</v>
       </c>
       <c r="N17">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="O17">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="P17">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -1376,46 +1373,46 @@
         <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C18">
-        <v>118.7</v>
+        <v>138</v>
       </c>
       <c r="D18">
-        <v>6.46</v>
+        <v>7</v>
       </c>
       <c r="E18">
-        <v>7.69</v>
+        <v>8.390000000000001</v>
       </c>
       <c r="F18">
-        <v>1.01</v>
+        <v>1.09</v>
       </c>
       <c r="G18">
-        <v>1690720000</v>
+        <v>2540090000</v>
       </c>
       <c r="H18">
-        <v>4834740</v>
+        <v>3523550</v>
       </c>
       <c r="I18">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="J18">
-        <v>3136.01</v>
+        <v>4569.92</v>
       </c>
       <c r="K18">
-        <v>298.55</v>
+        <v>391.42</v>
       </c>
       <c r="L18">
-        <v>9.52</v>
+        <v>8.57</v>
       </c>
       <c r="M18">
-        <v>0.42</v>
+        <v>1.1</v>
       </c>
       <c r="N18">
+        <v>21</v>
+      </c>
+      <c r="O18">
         <v>13</v>
-      </c>
-      <c r="O18">
-        <v>21</v>
       </c>
       <c r="P18">
         <v>34</v>
@@ -1429,46 +1426,46 @@
         <v>46</v>
       </c>
       <c r="C19">
-        <v>124.55</v>
+        <v>185.4</v>
       </c>
       <c r="D19">
-        <v>6.74</v>
+        <v>8.15</v>
       </c>
       <c r="E19">
-        <v>7.82</v>
+        <v>12.33</v>
       </c>
       <c r="F19">
-        <v>1.03</v>
+        <v>1.22</v>
       </c>
       <c r="G19">
-        <v>1840700000</v>
+        <v>278904000</v>
       </c>
       <c r="H19">
-        <v>3467620</v>
+        <v>2212560</v>
       </c>
       <c r="I19">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="J19">
-        <v>3869.34</v>
+        <v>377.76</v>
       </c>
       <c r="K19">
-        <v>374.15</v>
+        <v>28.08</v>
       </c>
       <c r="L19">
-        <v>9.67</v>
+        <v>7.43</v>
       </c>
       <c r="M19">
         <v>0</v>
       </c>
       <c r="N19">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="O19">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="P19">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1476,49 +1473,49 @@
         <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C20">
-        <v>137.83</v>
+        <v>119</v>
       </c>
       <c r="D20">
-        <v>7.01</v>
+        <v>6.44</v>
       </c>
       <c r="E20">
-        <v>8.4</v>
+        <v>7.67</v>
       </c>
       <c r="F20">
-        <v>1.11</v>
+        <v>1.03</v>
       </c>
       <c r="G20">
-        <v>2536960000</v>
+        <v>1695000000</v>
       </c>
       <c r="H20">
-        <v>3604760</v>
+        <v>4677020</v>
       </c>
       <c r="I20">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="J20">
-        <v>4698.17</v>
+        <v>3194.91</v>
       </c>
       <c r="K20">
-        <v>391.42</v>
+        <v>298.55</v>
       </c>
       <c r="L20">
-        <v>8.33</v>
+        <v>9.34</v>
       </c>
       <c r="M20">
-        <v>1.1</v>
+        <v>0.42</v>
       </c>
       <c r="N20">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O20">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="P20">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1529,46 +1526,46 @@
         <v>42</v>
       </c>
       <c r="C21">
-        <v>163.84</v>
+        <v>118</v>
       </c>
       <c r="D21">
-        <v>6.74</v>
+        <v>6.84</v>
       </c>
       <c r="E21">
-        <v>7.1</v>
+        <v>8.5</v>
       </c>
       <c r="F21">
-        <v>1.03</v>
+        <v>1.12</v>
       </c>
       <c r="G21">
-        <v>3957900000</v>
+        <v>1163530000</v>
       </c>
       <c r="H21">
-        <v>3854930</v>
+        <v>1595090</v>
       </c>
       <c r="I21">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="J21">
-        <v>5215.33</v>
+        <v>5937.55</v>
       </c>
       <c r="K21">
-        <v>396.01</v>
+        <v>377.38</v>
       </c>
       <c r="L21">
-        <v>7.59</v>
+        <v>6.36</v>
       </c>
       <c r="M21">
-        <v>0.21</v>
+        <v>3.2</v>
       </c>
       <c r="N21">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="O21">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="P21">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1576,49 +1573,49 @@
         <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C22">
-        <v>228.5</v>
+        <v>166.35</v>
       </c>
       <c r="D22">
-        <v>5.73</v>
+        <v>6.64</v>
       </c>
       <c r="E22">
-        <v>8.369999999999999</v>
+        <v>6.99</v>
       </c>
       <c r="F22">
-        <v>1.02</v>
+        <v>1.05</v>
       </c>
       <c r="G22">
-        <v>2908760000</v>
+        <v>4018540000</v>
       </c>
       <c r="H22">
-        <v>5039150</v>
+        <v>3831430</v>
       </c>
       <c r="I22">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="J22">
-        <v>5284.72</v>
+        <v>5327.09</v>
       </c>
       <c r="K22">
-        <v>316.98</v>
+        <v>396.01</v>
       </c>
       <c r="L22">
-        <v>6</v>
+        <v>7.43</v>
       </c>
       <c r="M22">
-        <v>5.97</v>
+        <v>0.21</v>
       </c>
       <c r="N22">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="O22">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="P22">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1629,46 +1626,46 @@
         <v>45</v>
       </c>
       <c r="C23">
-        <v>115.11</v>
+        <v>126.26</v>
       </c>
       <c r="D23">
-        <v>5.47</v>
+        <v>6.64</v>
       </c>
       <c r="E23">
-        <v>8.24</v>
+        <v>7.71</v>
       </c>
       <c r="F23">
-        <v>1.03</v>
+        <v>1.05</v>
       </c>
       <c r="G23">
-        <v>3547940000</v>
+        <v>1865970000</v>
       </c>
       <c r="H23">
-        <v>13273200</v>
+        <v>3404770</v>
       </c>
       <c r="I23">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J23">
-        <v>6493.88</v>
+        <v>3940.27</v>
       </c>
       <c r="K23">
-        <v>421.2</v>
+        <v>374.15</v>
       </c>
       <c r="L23">
-        <v>6.49</v>
+        <v>9.5</v>
       </c>
       <c r="M23">
         <v>0</v>
       </c>
       <c r="N23">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="O23">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="P23">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -1679,46 +1676,46 @@
         <v>42</v>
       </c>
       <c r="C24">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D24">
-        <v>6.78</v>
+        <v>5.81</v>
       </c>
       <c r="E24">
-        <v>6.77</v>
+        <v>9.09</v>
       </c>
       <c r="F24">
-        <v>1.12</v>
+        <v>1.04</v>
       </c>
       <c r="G24">
-        <v>934366000</v>
+        <v>2906250000</v>
       </c>
       <c r="H24">
-        <v>4068090</v>
+        <v>9183490</v>
       </c>
       <c r="I24">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J24">
-        <v>7803.63</v>
+        <v>5165</v>
       </c>
       <c r="K24">
-        <v>592.8200000000001</v>
+        <v>304.94</v>
       </c>
       <c r="L24">
-        <v>7.6</v>
+        <v>5.9</v>
       </c>
       <c r="M24">
-        <v>4.25</v>
+        <v>4.4</v>
       </c>
       <c r="N24">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="O24">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="P24">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -1729,46 +1726,46 @@
         <v>42</v>
       </c>
       <c r="C25">
-        <v>119.54</v>
+        <v>105.98</v>
       </c>
       <c r="D25">
-        <v>6.75</v>
+        <v>6.72</v>
       </c>
       <c r="E25">
-        <v>7.78</v>
+        <v>6.7</v>
       </c>
       <c r="F25">
-        <v>1.12</v>
+        <v>1.13</v>
       </c>
       <c r="G25">
-        <v>1178710000</v>
+        <v>943087000</v>
       </c>
       <c r="H25">
-        <v>1711970</v>
+        <v>4249250</v>
       </c>
       <c r="I25">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="J25">
-        <v>5927.09</v>
+        <v>7871.84</v>
       </c>
       <c r="K25">
-        <v>377.38</v>
+        <v>592.8200000000001</v>
       </c>
       <c r="L25">
-        <v>6.37</v>
+        <v>7.53</v>
       </c>
       <c r="M25">
-        <v>3.2</v>
+        <v>4.25</v>
       </c>
       <c r="N25">
         <v>23</v>
       </c>
       <c r="O25">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P25">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -1776,302 +1773,52 @@
         <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26">
-        <v>120.28</v>
+        <v>114.79</v>
       </c>
       <c r="D26">
-        <v>6.29</v>
+        <v>5.48</v>
       </c>
       <c r="E26">
-        <v>8.390000000000001</v>
+        <v>8.960000000000001</v>
       </c>
       <c r="F26">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="G26">
-        <v>2555190000</v>
+        <v>3538080000</v>
       </c>
       <c r="H26">
-        <v>5792610</v>
+        <v>14319700</v>
       </c>
       <c r="I26">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="J26">
-        <v>3806.63</v>
+        <v>6519.38</v>
       </c>
       <c r="K26">
-        <v>319.62</v>
+        <v>421.2</v>
       </c>
       <c r="L26">
-        <v>8.4</v>
+        <v>6.46</v>
       </c>
       <c r="M26">
-        <v>5.98</v>
+        <v>0</v>
       </c>
       <c r="N26">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="O26">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="P26">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16">
-      <c r="A27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27">
-        <v>104.01</v>
-      </c>
-      <c r="D27">
-        <v>5.7</v>
-      </c>
-      <c r="E27">
-        <v>8.210000000000001</v>
-      </c>
-      <c r="F27">
-        <v>1.05</v>
-      </c>
-      <c r="G27">
-        <v>2963520000</v>
-      </c>
-      <c r="H27">
-        <v>7724570</v>
-      </c>
-      <c r="I27">
-        <v>20</v>
-      </c>
-      <c r="J27">
-        <v>4301.6</v>
-      </c>
-      <c r="K27">
-        <v>304.94</v>
-      </c>
-      <c r="L27">
-        <v>7.09</v>
-      </c>
-      <c r="M27">
-        <v>4.4</v>
-      </c>
-      <c r="N27">
-        <v>19</v>
-      </c>
-      <c r="O27">
-        <v>24</v>
-      </c>
-      <c r="P27">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C1E5D1EB1B65964C845AF9732F46C499" ma:contentTypeVersion="9" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="53da220994c263061237558b4b19d7e9">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="94331225-a384-4379-98f7-51cdceba5e43" xmlns:ns3="2da23abd-c153-46ca-9656-d51f60595101" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9771c53ab827f697218d6811cc07834c" ns2:_="" ns3:_="">
-    <xsd:import namespace="94331225-a384-4379-98f7-51cdceba5e43"/>
-    <xsd:import namespace="2da23abd-c153-46ca-9656-d51f60595101"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="94331225-a384-4379-98f7-51cdceba5e43" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="12" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Marcações de imagem" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="e7912142-87f1-4323-af52-89749fe2aa64" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2da23abd-c153-46ca-9656-d51f60595101" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="13" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{7225a6a2-3862-4ca6-91e6-3196d49f2770}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="2da23abd-c153-46ca-9656-d51f60595101">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de Conteúdo"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3AB5599C-2336-4777-BBCE-8A720C0DDC0C}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D39F603-F797-444B-8472-EF6EFEB210A5}"/>
 </file>
</xml_diff>

<commit_message>
Atualização do "requirements.txt" e limpeza do código
</commit_message>
<xml_diff>
--- a/Fii_Tij_Hibrid_Mágicas.xlsx
+++ b/Fii_Tij_Hibrid_Mágicas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>Papel</t>
   </si>
@@ -64,106 +64,82 @@
     <t>Score</t>
   </si>
   <si>
-    <t>VINO11</t>
+    <t>MALL11</t>
+  </si>
+  <si>
+    <t>RZAT11</t>
+  </si>
+  <si>
+    <t>XPLG11</t>
+  </si>
+  <si>
+    <t>GGRC11</t>
+  </si>
+  <si>
+    <t>BRCO11</t>
+  </si>
+  <si>
+    <t>RBRP11</t>
+  </si>
+  <si>
+    <t>TVRI11</t>
+  </si>
+  <si>
+    <t>VISC11</t>
+  </si>
+  <si>
+    <t>LVBI11</t>
   </si>
   <si>
     <t>BRCR11</t>
   </si>
   <si>
-    <t>RZAT11</t>
-  </si>
-  <si>
-    <t>MALL11</t>
-  </si>
-  <si>
-    <t>VILG11</t>
-  </si>
-  <si>
-    <t>TVRI11</t>
-  </si>
-  <si>
-    <t>JSRE11</t>
-  </si>
-  <si>
-    <t>XPLG11</t>
-  </si>
-  <si>
-    <t>GGRC11</t>
+    <t>RCRB11</t>
+  </si>
+  <si>
+    <t>TGAR11</t>
+  </si>
+  <si>
+    <t>TRXF11</t>
+  </si>
+  <si>
+    <t>RBVA11</t>
+  </si>
+  <si>
+    <t>HGRU11</t>
+  </si>
+  <si>
+    <t>XPML11</t>
+  </si>
+  <si>
+    <t>ALZR11</t>
   </si>
   <si>
     <t>HSML11</t>
   </si>
   <si>
-    <t>TGAR11</t>
-  </si>
-  <si>
-    <t>RBVA11</t>
-  </si>
-  <si>
-    <t>RCRB11</t>
-  </si>
-  <si>
-    <t>FATN11</t>
-  </si>
-  <si>
-    <t>TRXF11</t>
-  </si>
-  <si>
-    <t>VISC11</t>
-  </si>
-  <si>
-    <t>LVBI11</t>
-  </si>
-  <si>
-    <t>HGBS11</t>
-  </si>
-  <si>
-    <t>GALG11</t>
-  </si>
-  <si>
-    <t>BRCO11</t>
+    <t>KNRI11</t>
   </si>
   <si>
     <t>BTLG11</t>
   </si>
   <si>
-    <t>HGRU11</t>
-  </si>
-  <si>
-    <t>ALZR11</t>
-  </si>
-  <si>
-    <t>KNRI11</t>
-  </si>
-  <si>
-    <t>PVBI11</t>
-  </si>
-  <si>
-    <t>HTMX11</t>
-  </si>
-  <si>
     <t>HSRE11</t>
   </si>
   <si>
-    <t>XPML11</t>
+    <t>Shoppings</t>
+  </si>
+  <si>
+    <t>Híbrido</t>
+  </si>
+  <si>
+    <t>Logística</t>
+  </si>
+  <si>
+    <t>Outros</t>
   </si>
   <si>
     <t>Lajes Corporativas</t>
-  </si>
-  <si>
-    <t>Híbrido</t>
-  </si>
-  <si>
-    <t>Shoppings</t>
-  </si>
-  <si>
-    <t>Logística</t>
-  </si>
-  <si>
-    <t>Outros</t>
-  </si>
-  <si>
-    <t>Hotel</t>
   </si>
 </sst>
 </file>
@@ -521,7 +497,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -582,49 +558,49 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C2">
-        <v>7.51</v>
+        <v>108.66</v>
       </c>
       <c r="D2">
-        <v>9.91</v>
+        <v>16.7</v>
       </c>
       <c r="E2">
-        <v>9.18</v>
+        <v>9.02</v>
       </c>
       <c r="F2">
-        <v>0.6899999999999999</v>
+        <v>0.91</v>
       </c>
       <c r="G2">
-        <v>622025000</v>
+        <v>1409640000</v>
       </c>
       <c r="H2">
-        <v>1319690</v>
+        <v>3328720</v>
       </c>
       <c r="I2">
         <v>10</v>
       </c>
       <c r="J2">
-        <v>9705.709999999999</v>
+        <v>4426.33</v>
       </c>
       <c r="K2">
-        <v>1189.57</v>
+        <v>473.96</v>
       </c>
       <c r="L2">
-        <v>12.26</v>
+        <v>10.71</v>
       </c>
       <c r="M2">
+        <v>3.64</v>
+      </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+      <c r="O2">
         <v>0</v>
       </c>
-      <c r="N2">
-        <v>2</v>
-      </c>
-      <c r="O2">
-        <v>3</v>
-      </c>
       <c r="P2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -632,49 +608,49 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C3">
-        <v>59.06</v>
+        <v>94.5</v>
       </c>
       <c r="D3">
-        <v>8.82</v>
+        <v>12.42</v>
       </c>
       <c r="E3">
-        <v>9.1</v>
+        <v>11.91</v>
       </c>
       <c r="F3">
-        <v>0.6</v>
+        <v>0.93</v>
       </c>
       <c r="G3">
-        <v>1573250000</v>
+        <v>350422000</v>
       </c>
       <c r="H3">
-        <v>1867970</v>
+        <v>1083690</v>
       </c>
       <c r="I3">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J3">
-        <v>44864.3</v>
+        <v>1328.95</v>
       </c>
       <c r="K3">
-        <v>5308.12</v>
+        <v>124.53</v>
       </c>
       <c r="L3">
-        <v>11.83</v>
+        <v>9.369999999999999</v>
       </c>
       <c r="M3">
-        <v>5.43</v>
+        <v>3.74</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P3">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -682,49 +658,49 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C4">
-        <v>95.64</v>
+        <v>102.67</v>
       </c>
       <c r="D4">
-        <v>12.24</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="E4">
-        <v>13.16</v>
+        <v>7.99</v>
       </c>
       <c r="F4">
-        <v>0.9399999999999999</v>
+        <v>0.92</v>
       </c>
       <c r="G4">
-        <v>354649000</v>
+        <v>3040390000</v>
       </c>
       <c r="H4">
-        <v>1196410</v>
+        <v>4708570</v>
       </c>
       <c r="I4">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="J4">
-        <v>1139.04</v>
+        <v>2325.15</v>
       </c>
       <c r="K4">
-        <v>115.13</v>
+        <v>219.61</v>
       </c>
       <c r="L4">
-        <v>10.11</v>
+        <v>9.44</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>4.11</v>
       </c>
       <c r="N4">
         <v>6</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P4">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -732,49 +708,49 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C5">
-        <v>118.46</v>
+        <v>10.86</v>
       </c>
       <c r="D5">
-        <v>18.32</v>
+        <v>9.279999999999999</v>
       </c>
       <c r="E5">
-        <v>7.89</v>
+        <v>10.59</v>
       </c>
       <c r="F5">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
       <c r="G5">
-        <v>1080910000</v>
+        <v>990449000</v>
       </c>
       <c r="H5">
-        <v>1988000</v>
+        <v>1322810</v>
       </c>
       <c r="I5">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="J5">
-        <v>4602.86</v>
+        <v>1036.39</v>
       </c>
       <c r="K5">
-        <v>697.37</v>
+        <v>107.81</v>
       </c>
       <c r="L5">
-        <v>15.15</v>
+        <v>10.4</v>
       </c>
       <c r="M5">
-        <v>3.67</v>
+        <v>0</v>
       </c>
       <c r="N5">
         <v>9</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P5">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -782,49 +758,49 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C6">
-        <v>91.33</v>
+        <v>109.88</v>
       </c>
       <c r="D6">
-        <v>7.94</v>
+        <v>7.03</v>
       </c>
       <c r="E6">
-        <v>8.31</v>
+        <v>9.26</v>
       </c>
       <c r="F6">
-        <v>0.8</v>
+        <v>0.92</v>
       </c>
       <c r="G6">
-        <v>1369710000</v>
+        <v>1745200000</v>
       </c>
       <c r="H6">
-        <v>2720940</v>
+        <v>3064700</v>
       </c>
       <c r="I6">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J6">
-        <v>2382.19</v>
+        <v>3443.91</v>
       </c>
       <c r="K6">
-        <v>235.99</v>
+        <v>375.46</v>
       </c>
       <c r="L6">
-        <v>9.91</v>
+        <v>10.9</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O6">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="P6">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -832,49 +808,49 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C7">
-        <v>101.4</v>
+        <v>56.77</v>
       </c>
       <c r="D7">
-        <v>10.51</v>
+        <v>5.27</v>
       </c>
       <c r="E7">
-        <v>3.56</v>
+        <v>7.6</v>
       </c>
       <c r="F7">
-        <v>1.01</v>
+        <v>0.71</v>
       </c>
       <c r="G7">
-        <v>1614260000</v>
+        <v>691412000</v>
       </c>
       <c r="H7">
-        <v>1542970</v>
+        <v>1546150</v>
       </c>
       <c r="I7">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="J7">
-        <v>4037.81</v>
+        <v>7761.44</v>
       </c>
       <c r="K7">
-        <v>487.92</v>
+        <v>507.95</v>
       </c>
       <c r="L7">
-        <v>12.08</v>
+        <v>6.54</v>
       </c>
       <c r="M7">
-        <v>1.45</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="O7">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="P7">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -882,49 +858,49 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C8">
-        <v>75.02</v>
+        <v>101.4</v>
       </c>
       <c r="D8">
-        <v>6.68</v>
+        <v>10.37</v>
       </c>
       <c r="E8">
-        <v>7.07</v>
+        <v>7.17</v>
       </c>
       <c r="F8">
-        <v>0.68</v>
+        <v>1.01</v>
       </c>
       <c r="G8">
-        <v>1557960000</v>
+        <v>1614260000</v>
       </c>
       <c r="H8">
-        <v>2509320</v>
+        <v>1208660</v>
       </c>
       <c r="I8">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="J8">
-        <v>13237</v>
+        <v>4063.88</v>
       </c>
       <c r="K8">
-        <v>1045.86</v>
+        <v>498.9</v>
       </c>
       <c r="L8">
-        <v>7.9</v>
+        <v>12.28</v>
       </c>
       <c r="M8">
-        <v>6.86</v>
+        <v>3.14</v>
       </c>
       <c r="N8">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="O8">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="P8">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -932,49 +908,49 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C9">
-        <v>111.3</v>
+        <v>111.99</v>
       </c>
       <c r="D9">
-        <v>7.92</v>
+        <v>5.89</v>
       </c>
       <c r="E9">
-        <v>7.23</v>
+        <v>9.779999999999999</v>
       </c>
       <c r="F9">
-        <v>0.99</v>
+        <v>0.88</v>
       </c>
       <c r="G9">
-        <v>3295950000</v>
+        <v>3228520000</v>
       </c>
       <c r="H9">
-        <v>6706800</v>
+        <v>8267000</v>
       </c>
       <c r="I9">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="J9">
-        <v>2493.87</v>
+        <v>3400.36</v>
       </c>
       <c r="K9">
-        <v>214.25</v>
+        <v>275.14</v>
       </c>
       <c r="L9">
-        <v>8.59</v>
+        <v>8.09</v>
       </c>
       <c r="M9">
-        <v>2.26</v>
+        <v>5.88</v>
       </c>
       <c r="N9">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="O9">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="P9">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -982,49 +958,49 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C10">
-        <v>113.85</v>
+        <v>111.83</v>
       </c>
       <c r="D10">
-        <v>8.369999999999999</v>
+        <v>6.84</v>
       </c>
       <c r="E10">
-        <v>10.35</v>
+        <v>8.91</v>
       </c>
       <c r="F10">
-        <v>1.01</v>
+        <v>0.96</v>
       </c>
       <c r="G10">
-        <v>1028200000</v>
+        <v>1802540000</v>
       </c>
       <c r="H10">
-        <v>1297230</v>
+        <v>4018880</v>
       </c>
       <c r="I10">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="J10">
-        <v>1166</v>
+        <v>2508.3</v>
       </c>
       <c r="K10">
-        <v>112.93</v>
+        <v>250.9</v>
       </c>
       <c r="L10">
-        <v>9.68</v>
+        <v>10</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>3.93</v>
       </c>
       <c r="N10">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="O10">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="P10">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1032,49 +1008,49 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C11">
-        <v>96.5</v>
+        <v>52.93</v>
       </c>
       <c r="D11">
-        <v>8.74</v>
+        <v>1.6</v>
       </c>
       <c r="E11">
-        <v>8.76</v>
+        <v>9.74</v>
       </c>
       <c r="F11">
-        <v>1.03</v>
+        <v>0.58</v>
       </c>
       <c r="G11">
-        <v>1522830000</v>
+        <v>1409960000</v>
       </c>
       <c r="H11">
-        <v>3358040</v>
+        <v>1703860</v>
       </c>
       <c r="I11">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J11">
-        <v>10380.1</v>
+        <v>9254.299999999999</v>
       </c>
       <c r="K11">
-        <v>864.59</v>
+        <v>1278.12</v>
       </c>
       <c r="L11">
-        <v>8.33</v>
+        <v>13.81</v>
       </c>
       <c r="M11">
-        <v>2.82</v>
+        <v>5.71</v>
       </c>
       <c r="N11">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="O11">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="P11">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1082,49 +1058,49 @@
         <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C12">
-        <v>126.7</v>
+        <v>145.99</v>
       </c>
       <c r="D12">
-        <v>9.449999999999999</v>
+        <v>2.97</v>
       </c>
       <c r="E12">
-        <v>12.96</v>
+        <v>7.24</v>
       </c>
       <c r="F12">
-        <v>1.04</v>
+        <v>0.71</v>
       </c>
       <c r="G12">
-        <v>2427650000</v>
+        <v>538805000</v>
       </c>
       <c r="H12">
-        <v>8082820</v>
+        <v>1096280</v>
       </c>
       <c r="I12">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J12">
-        <v>76.26000000000001</v>
+        <v>13199</v>
       </c>
       <c r="K12">
-        <v>1.8</v>
+        <v>1097.8</v>
       </c>
       <c r="L12">
-        <v>2.36</v>
+        <v>8.32</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>3.61</v>
       </c>
       <c r="N12">
+        <v>2</v>
+      </c>
+      <c r="O12">
+        <v>19</v>
+      </c>
+      <c r="P12">
         <v>21</v>
-      </c>
-      <c r="O12">
-        <v>4</v>
-      </c>
-      <c r="P12">
-        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1132,49 +1108,49 @@
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C13">
-        <v>113.25</v>
+        <v>123.1</v>
       </c>
       <c r="D13">
-        <v>8.82</v>
+        <v>10.38</v>
       </c>
       <c r="E13">
-        <v>10.66</v>
+        <v>12.42</v>
       </c>
       <c r="F13">
-        <v>1.04</v>
+        <v>1.05</v>
       </c>
       <c r="G13">
-        <v>1413960000</v>
+        <v>2358670000</v>
       </c>
       <c r="H13">
-        <v>1488190</v>
+        <v>6667580</v>
       </c>
       <c r="I13">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="J13">
-        <v>17569.7</v>
+        <v>77.51000000000001</v>
       </c>
       <c r="K13">
-        <v>1947.03</v>
+        <v>1.36</v>
       </c>
       <c r="L13">
-        <v>11.08</v>
+        <v>1.75</v>
       </c>
       <c r="M13">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="N13">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P13">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1182,49 +1158,49 @@
         <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C14">
-        <v>163.32</v>
+        <v>105.55</v>
       </c>
       <c r="D14">
-        <v>5.1</v>
+        <v>7.33</v>
       </c>
       <c r="E14">
-        <v>6.02</v>
+        <v>10.36</v>
       </c>
       <c r="F14">
-        <v>0.79</v>
+        <v>0.99</v>
       </c>
       <c r="G14">
-        <v>602764000</v>
+        <v>1622540000</v>
       </c>
       <c r="H14">
-        <v>1000540</v>
+        <v>7754020</v>
       </c>
       <c r="I14">
+        <v>29</v>
+      </c>
+      <c r="J14">
+        <v>3146.81</v>
+      </c>
+      <c r="K14">
+        <v>347.9</v>
+      </c>
+      <c r="L14">
+        <v>11.06</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>13</v>
+      </c>
+      <c r="O14">
         <v>9</v>
       </c>
-      <c r="J14">
-        <v>14742.8</v>
-      </c>
-      <c r="K14">
-        <v>1055.21</v>
-      </c>
-      <c r="L14">
-        <v>7.16</v>
-      </c>
-      <c r="M14">
-        <v>6.71</v>
-      </c>
-      <c r="N14">
-        <v>3</v>
-      </c>
-      <c r="O14">
-        <v>25</v>
-      </c>
       <c r="P14">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1232,49 +1208,49 @@
         <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C15">
-        <v>91.8</v>
+        <v>109.2</v>
       </c>
       <c r="D15">
-        <v>5.53</v>
+        <v>8.51</v>
       </c>
       <c r="E15">
-        <v>11.16</v>
+        <v>11.21</v>
       </c>
       <c r="F15">
-        <v>0.89</v>
+        <v>1.01</v>
       </c>
       <c r="G15">
-        <v>268500000</v>
+        <v>1363400000</v>
       </c>
       <c r="H15">
-        <v>1403350</v>
+        <v>1651330</v>
       </c>
       <c r="I15">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="J15">
-        <v>24130.2</v>
+        <v>17442.4</v>
       </c>
       <c r="K15">
-        <v>1489.85</v>
+        <v>1975.52</v>
       </c>
       <c r="L15">
-        <v>6.17</v>
+        <v>11.33</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>0.43</v>
       </c>
       <c r="N15">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="O15">
+        <v>6</v>
+      </c>
+      <c r="P15">
         <v>23</v>
-      </c>
-      <c r="P15">
-        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1282,49 +1258,49 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C16">
-        <v>112.27</v>
+        <v>127.1</v>
       </c>
       <c r="D16">
-        <v>6.89</v>
+        <v>7.66</v>
       </c>
       <c r="E16">
-        <v>9.59</v>
+        <v>9.140000000000001</v>
       </c>
       <c r="F16">
-        <v>1.03</v>
+        <v>1.01</v>
       </c>
       <c r="G16">
-        <v>1725840000</v>
+        <v>2339460000</v>
       </c>
       <c r="H16">
-        <v>10730600</v>
+        <v>3501990</v>
       </c>
       <c r="I16">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="J16">
-        <v>3377.69</v>
+        <v>4535.68</v>
       </c>
       <c r="K16">
-        <v>344.45</v>
+        <v>421.38</v>
       </c>
       <c r="L16">
-        <v>10.2</v>
+        <v>9.289999999999999</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>0.97</v>
       </c>
       <c r="N16">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="O16">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="P16">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1332,49 +1308,49 @@
         <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C17">
-        <v>121.5</v>
+        <v>110.86</v>
       </c>
       <c r="D17">
-        <v>4.94</v>
+        <v>7.15</v>
       </c>
       <c r="E17">
-        <v>8.449999999999999</v>
+        <v>8.98</v>
       </c>
       <c r="F17">
-        <v>0.9399999999999999</v>
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>3502680000</v>
+        <v>4407570000</v>
       </c>
       <c r="H17">
-        <v>10514700</v>
+        <v>17480800</v>
       </c>
       <c r="I17">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J17">
-        <v>3484.68</v>
+        <v>6047.65</v>
       </c>
       <c r="K17">
-        <v>269.97</v>
+        <v>448.85</v>
       </c>
       <c r="L17">
-        <v>7.75</v>
+        <v>7.42</v>
       </c>
       <c r="M17">
-        <v>4.74</v>
+        <v>0.23</v>
       </c>
       <c r="N17">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="O17">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="P17">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -1382,49 +1358,49 @@
         <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C18">
-        <v>118.49</v>
+        <v>109.06</v>
       </c>
       <c r="D18">
-        <v>6.21</v>
+        <v>8.27</v>
       </c>
       <c r="E18">
-        <v>7.94</v>
+        <v>8.35</v>
       </c>
       <c r="F18">
-        <v>1.01</v>
+        <v>1.03</v>
       </c>
       <c r="G18">
-        <v>1687730000</v>
+        <v>1075380000</v>
       </c>
       <c r="H18">
-        <v>4650790</v>
+        <v>2270850</v>
       </c>
       <c r="I18">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J18">
-        <v>3237.6</v>
+        <v>5328.98</v>
       </c>
       <c r="K18">
-        <v>308.2</v>
+        <v>410.01</v>
       </c>
       <c r="L18">
-        <v>9.52</v>
+        <v>7.69</v>
       </c>
       <c r="M18">
-        <v>0.43</v>
+        <v>0</v>
       </c>
       <c r="N18">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="O18">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="P18">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -1432,49 +1408,49 @@
         <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C19">
-        <v>231.9</v>
+        <v>95.34999999999999</v>
       </c>
       <c r="D19">
-        <v>5.98</v>
+        <v>6.63</v>
       </c>
       <c r="E19">
-        <v>8.390000000000001</v>
+        <v>9.109999999999999</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="G19">
-        <v>2952040000</v>
+        <v>1946870000</v>
       </c>
       <c r="H19">
-        <v>5780500</v>
+        <v>4543960</v>
       </c>
       <c r="I19">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="J19">
-        <v>4908.72</v>
+        <v>9603.629999999999</v>
       </c>
       <c r="K19">
-        <v>302.79</v>
+        <v>898.7</v>
       </c>
       <c r="L19">
-        <v>6.17</v>
+        <v>9.359999999999999</v>
       </c>
       <c r="M19">
-        <v>5.37</v>
+        <v>5.02</v>
       </c>
       <c r="N19">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O19">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="P19">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1482,49 +1458,49 @@
         <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C20">
-        <v>9.08</v>
+        <v>155.65</v>
       </c>
       <c r="D20">
-        <v>3.87</v>
+        <v>5.78</v>
       </c>
       <c r="E20">
-        <v>9.48</v>
+        <v>7.63</v>
       </c>
       <c r="F20">
         <v>0.98</v>
       </c>
       <c r="G20">
-        <v>1142860000</v>
+        <v>4390660000</v>
       </c>
       <c r="H20">
-        <v>2869930</v>
+        <v>4164110</v>
       </c>
       <c r="I20">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="J20">
-        <v>5315.38</v>
+        <v>4992.48</v>
       </c>
       <c r="K20">
-        <v>492.6</v>
+        <v>371.22</v>
       </c>
       <c r="L20">
-        <v>9.27</v>
+        <v>7.44</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="N20">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="O20">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="P20">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1532,49 +1508,49 @@
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C21">
-        <v>123.74</v>
+        <v>99</v>
       </c>
       <c r="D21">
-        <v>6.33</v>
+        <v>4.42</v>
       </c>
       <c r="E21">
-        <v>8.06</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="F21">
-        <v>1.03</v>
+        <v>0.99</v>
       </c>
       <c r="G21">
-        <v>1828730000</v>
+        <v>4281670000</v>
       </c>
       <c r="H21">
-        <v>3031190</v>
+        <v>9666930</v>
       </c>
       <c r="I21">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="J21">
-        <v>3862.98</v>
+        <v>3216.37</v>
       </c>
       <c r="K21">
-        <v>366</v>
+        <v>213.45</v>
       </c>
       <c r="L21">
-        <v>9.470000000000001</v>
+        <v>6.64</v>
       </c>
       <c r="M21">
-        <v>0</v>
+        <v>2.43</v>
       </c>
       <c r="N21">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="O21">
         <v>18</v>
       </c>
       <c r="P21">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1582,399 +1558,49 @@
         <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C22">
-        <v>103.3</v>
+        <v>108.99</v>
       </c>
       <c r="D22">
-        <v>6.33</v>
+        <v>6.53</v>
       </c>
       <c r="E22">
-        <v>9</v>
+        <v>6.62</v>
       </c>
       <c r="F22">
-        <v>1.03</v>
+        <v>1.15</v>
       </c>
       <c r="G22">
-        <v>2943290000</v>
+        <v>969872000</v>
       </c>
       <c r="H22">
-        <v>10350400</v>
+        <v>2662050</v>
       </c>
       <c r="I22">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="J22">
-        <v>1267.46</v>
+        <v>7993.47</v>
       </c>
       <c r="K22">
-        <v>77.14</v>
+        <v>628.24</v>
       </c>
       <c r="L22">
-        <v>6.09</v>
+        <v>7.86</v>
       </c>
       <c r="M22">
-        <v>0.74</v>
+        <v>1.21</v>
       </c>
       <c r="N22">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="O22">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="P22">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16">
-      <c r="A23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23">
-        <v>136.4</v>
-      </c>
-      <c r="D23">
-        <v>7.16</v>
-      </c>
-      <c r="E23">
-        <v>8.51</v>
-      </c>
-      <c r="F23">
-        <v>1.08</v>
-      </c>
-      <c r="G23">
-        <v>2510640000</v>
-      </c>
-      <c r="H23">
-        <v>3537520</v>
-      </c>
-      <c r="I23">
-        <v>69</v>
-      </c>
-      <c r="J23">
-        <v>4815.42</v>
-      </c>
-      <c r="K23">
-        <v>422.51</v>
-      </c>
-      <c r="L23">
-        <v>8.77</v>
-      </c>
-      <c r="M23">
-        <v>0.97</v>
-      </c>
-      <c r="N23">
-        <v>25</v>
-      </c>
-      <c r="O23">
-        <v>12</v>
-      </c>
-      <c r="P23">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16">
-      <c r="A24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24">
-        <v>117.3</v>
-      </c>
-      <c r="D24">
-        <v>7.34</v>
-      </c>
-      <c r="E24">
-        <v>8.58</v>
-      </c>
-      <c r="F24">
-        <v>1.1</v>
-      </c>
-      <c r="G24">
-        <v>1156630000</v>
-      </c>
-      <c r="H24">
-        <v>1666220</v>
-      </c>
-      <c r="I24">
-        <v>14</v>
-      </c>
-      <c r="J24">
-        <v>5536.27</v>
-      </c>
-      <c r="K24">
-        <v>382.83</v>
-      </c>
-      <c r="L24">
-        <v>6.91</v>
-      </c>
-      <c r="M24">
-        <v>3.03</v>
-      </c>
-      <c r="N24">
-        <v>26</v>
-      </c>
-      <c r="O24">
-        <v>11</v>
-      </c>
-      <c r="P24">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
-      <c r="A25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25">
-        <v>165.36</v>
-      </c>
-      <c r="D25">
-        <v>6.6</v>
-      </c>
-      <c r="E25">
-        <v>7.09</v>
-      </c>
-      <c r="F25">
-        <v>1.04</v>
-      </c>
-      <c r="G25">
-        <v>3994620000</v>
-      </c>
-      <c r="H25">
-        <v>3899680</v>
-      </c>
-      <c r="I25">
-        <v>19</v>
-      </c>
-      <c r="J25">
-        <v>5266.55</v>
-      </c>
-      <c r="K25">
-        <v>383.4</v>
-      </c>
-      <c r="L25">
-        <v>7.28</v>
-      </c>
-      <c r="M25">
-        <v>0.18</v>
-      </c>
-      <c r="N25">
-        <v>22</v>
-      </c>
-      <c r="O25">
-        <v>16</v>
-      </c>
-      <c r="P25">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
-      <c r="A26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26">
-        <v>103.02</v>
-      </c>
-      <c r="D26">
-        <v>5.44</v>
-      </c>
-      <c r="E26">
-        <v>7.37</v>
-      </c>
-      <c r="F26">
-        <v>1.02</v>
-      </c>
-      <c r="G26">
-        <v>1896830000</v>
-      </c>
-      <c r="H26">
-        <v>4976720</v>
-      </c>
-      <c r="I26">
-        <v>5</v>
-      </c>
-      <c r="J26">
-        <v>23767</v>
-      </c>
-      <c r="K26">
-        <v>1166.96</v>
-      </c>
-      <c r="L26">
-        <v>4.91</v>
-      </c>
-      <c r="M26">
-        <v>0.84</v>
-      </c>
-      <c r="N26">
-        <v>15</v>
-      </c>
-      <c r="O26">
-        <v>24</v>
-      </c>
-      <c r="P26">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16">
-      <c r="A27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27">
-        <v>158.94</v>
-      </c>
-      <c r="D27">
-        <v>6.37</v>
-      </c>
-      <c r="E27">
-        <v>14.46</v>
-      </c>
-      <c r="F27">
-        <v>1.07</v>
-      </c>
-      <c r="G27">
-        <v>239099000</v>
-      </c>
-      <c r="H27">
-        <v>2575940</v>
-      </c>
-      <c r="I27">
-        <v>22</v>
-      </c>
-      <c r="J27">
-        <v>300325</v>
-      </c>
-      <c r="K27">
-        <v>27808.37</v>
-      </c>
-      <c r="L27">
-        <v>9.26</v>
-      </c>
-      <c r="M27">
-        <v>3.46</v>
-      </c>
-      <c r="N27">
-        <v>24</v>
-      </c>
-      <c r="O27">
-        <v>17</v>
-      </c>
-      <c r="P27">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16">
-      <c r="A28" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28">
-        <v>106.27</v>
-      </c>
-      <c r="D28">
-        <v>6.81</v>
-      </c>
-      <c r="E28">
-        <v>6.66</v>
-      </c>
-      <c r="F28">
-        <v>1.13</v>
-      </c>
-      <c r="G28">
-        <v>945667000</v>
-      </c>
-      <c r="H28">
-        <v>2400840</v>
-      </c>
-      <c r="I28">
-        <v>27</v>
-      </c>
-      <c r="J28">
-        <v>8139.14</v>
-      </c>
-      <c r="K28">
-        <v>616.51</v>
-      </c>
-      <c r="L28">
-        <v>7.57</v>
-      </c>
-      <c r="M28">
-        <v>1.21</v>
-      </c>
-      <c r="N28">
-        <v>27</v>
-      </c>
-      <c r="O28">
-        <v>14</v>
-      </c>
-      <c r="P28">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16">
-      <c r="A29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29">
-        <v>117.73</v>
-      </c>
-      <c r="D29">
-        <v>6.31</v>
-      </c>
-      <c r="E29">
-        <v>8.75</v>
-      </c>
-      <c r="F29">
-        <v>1.05</v>
-      </c>
-      <c r="G29">
-        <v>3628700000</v>
-      </c>
-      <c r="H29">
-        <v>14338300</v>
-      </c>
-      <c r="I29">
-        <v>14</v>
-      </c>
-      <c r="J29">
-        <v>5940.76</v>
-      </c>
-      <c r="K29">
-        <v>358.17</v>
-      </c>
-      <c r="L29">
-        <v>6.03</v>
-      </c>
-      <c r="M29">
-        <v>5.32</v>
-      </c>
-      <c r="N29">
-        <v>23</v>
-      </c>
-      <c r="O29">
-        <v>20</v>
-      </c>
-      <c r="P29">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2181,9 +1807,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C94F2794-98AF-42A1-B268-70C4E32B8915}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3874B947-B99D-4396-8F2D-EA300FAE73B0}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C3678A8-602D-41DA-BAEC-E13CED9BDA9E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0463F97-040B-49C3-934C-1828789B87BE}"/>
 </file>
</xml_diff>